<commit_message>
update to publish v1.8.7
</commit_message>
<xml_diff>
--- a/ig/clcore/1.8.6/ValueSet-VSDiagnosticosSCT.xlsx
+++ b/ig/clcore/1.8.6/ValueSet-VSDiagnosticosSCT.xlsx
@@ -8,7 +8,7 @@
   <sheets>
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
     <sheet name="Include from SNOMED CT" r:id="rId4" sheetId="2"/>
-    <sheet name="Include from absent-unknown-u" r:id="rId5" sheetId="3"/>
+    <sheet name="Include from CodeSystem-absen" r:id="rId5" sheetId="3"/>
   </sheets>
 </workbook>
 </file>
@@ -118,7 +118,7 @@
     <t>http://snomed.info/sct</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/uv/ips/CodeSystem/absent-unknown-uv-ips</t>
+    <t>https://hl7.org/fhir/uv/ips/STU1.1/CodeSystem-absent-unknown-uv-ips.html</t>
   </si>
 </sst>
 </file>

</xml_diff>